<commit_message>
Feat: Integrando notificacio de carga de reporte y selector de periodos para la actividad del empleado
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -419,44 +419,38 @@
         <v>tipoMantenimiento</v>
       </c>
       <c r="F1" t="str">
-        <v>estadoUnidad</v>
+        <v>estadoEntrega</v>
       </c>
       <c r="G1" t="str">
-        <v>estadoEntrega</v>
-      </c>
-      <c r="H1" t="str">
         <v>comment</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Amayrani Ayala</v>
+        <v xml:space="preserve">RIKO VIX </v>
       </c>
       <c r="B2" t="str">
-        <v>TC-115</v>
+        <v>123</v>
       </c>
       <c r="C2" t="str">
-        <v>Basé Cuautitlan Izcalli</v>
+        <v>CDMX</v>
       </c>
       <c r="D2" t="str">
-        <v>Base</v>
+        <v>Bodega</v>
       </c>
       <c r="E2" t="str">
-        <v>Preventivo</v>
+        <v>Correctivo</v>
       </c>
       <c r="F2" t="str">
-        <v/>
+        <v>Estaba por entregar</v>
       </c>
       <c r="G2" t="str">
-        <v/>
-      </c>
-      <c r="H2" t="str">
-        <v>Manguera sin sello plastico</v>
+        <v>se chingo una llanta</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>